<commit_message>
MNT/SM: Add setting files for 129Xe27 to 50 from MEBT to FS1A,B, FS2.
</commit_message>
<xml_diff>
--- a/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/ARR04_2020Oct_ver20201005.xlsx
+++ b/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/ARR04_2020Oct_ver20201005.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="143">
   <si>
     <t xml:space="preserve">MEBT to FS1A</t>
   </si>
@@ -446,6 +446,30 @@
   </si>
   <si>
     <t xml:space="preserve">Q_D4000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">129Xe27+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">to 50+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">129Xe27+ to 50+</t>
   </si>
 </sst>
 </file>
@@ -456,7 +480,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -478,6 +502,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -522,12 +552,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,9 +588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>570240</xdr:colOff>
+      <xdr:colOff>569880</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -569,8 +603,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3055680" y="1827360"/>
-          <a:ext cx="5352840" cy="5096160"/>
+          <a:off x="3843360" y="1827360"/>
+          <a:ext cx="6612480" cy="5095800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -586,7 +620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -596,10 +630,11 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.55"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,17 +2468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CG5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +2735,6 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>83</v>
@@ -2968,17 +3005,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,10 +3282,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>91</v>
+    <row r="4" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>16.5</v>
@@ -3519,17 +3559,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:ED4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3930,10 +3974,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>180</v>

</xml_diff>